<commit_message>
Added trigger TODOs + added urlPhoto field in DB script
</commit_message>
<xml_diff>
--- a/SQL/PICTURA_SQLPlan.xlsx
+++ b/SQL/PICTURA_SQLPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephane\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdema\switchdrive\HEIG-VD\BDR\Projet\App\BDR_PICTURA\SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1202789B-FCF8-4E4F-86CA-9F00B92A0F5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C375D5-FA37-413A-B094-F838B70D195C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SQLQueries" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
   <si>
     <t>Action</t>
   </si>
@@ -168,13 +168,31 @@
   </si>
   <si>
     <t>Event</t>
+  </si>
+  <si>
+    <t>delete tag if no photo uses it anymore</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>comment only responds to comments on same photo</t>
+  </si>
+  <si>
+    <t>response's datetime &gt; parent comment</t>
+  </si>
+  <si>
+    <t>comment datetime &gt; photo datetime</t>
+  </si>
+  <si>
+    <t>there must always be one admin per community</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,8 +224,15 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,6 +251,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -236,16 +266,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -274,8 +302,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
@@ -307,11 +342,11 @@
       <font>
         <b/>
         <i val="0"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF9F9F"/>
+          <bgColor rgb="FFB6DF89"/>
         </patternFill>
       </fill>
     </dxf>
@@ -319,11 +354,11 @@
       <font>
         <b/>
         <i val="0"/>
-        <color rgb="FF00B050"/>
+        <color rgb="FFFF0000"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFB6DF89"/>
+          <bgColor rgb="FFFF9F9F"/>
         </patternFill>
       </fill>
     </dxf>
@@ -635,280 +670,280 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="40.77734375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="40.77734375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="C3" s="2" t="s">
+    <row r="3" spans="3:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C4" s="4" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C5" s="5" t="s">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C6" s="5" t="s">
+    <row r="6" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C7" s="5" t="s">
+    <row r="7" spans="3:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C8" s="5" t="s">
+    <row r="8" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="5" t="s">
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C10" s="5" t="s">
+    <row r="10" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="3:6" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="C11" s="5" t="s">
+    <row r="11" spans="3:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="C11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="3:6" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="C12" s="5" t="s">
+    <row r="12" spans="3:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="C12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="3:6" ht="79.2" x14ac:dyDescent="0.3">
-      <c r="C13" s="5" t="s">
+    <row r="13" spans="3:6" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="C13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="3:6" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="C14" s="5" t="s">
+    <row r="14" spans="3:6" ht="51" x14ac:dyDescent="0.25">
+      <c r="C14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="5" t="s">
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C16" s="5" t="s">
+    <row r="16" spans="3:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="C16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C17" s="5" t="s">
+    <row r="17" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C18" s="5" t="s">
+    <row r="18" spans="3:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C19" s="5" t="s">
+    <row r="19" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C20" s="5" t="s">
+    <row r="20" spans="3:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C21" s="5" t="s">
+    <row r="21" spans="3:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="C21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C22" s="5" t="s">
+    <row r="22" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C22" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F22" s="1" t="s">
@@ -936,61 +971,101 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E5BF619-A8CD-4AA9-8EE1-02874CED833F}">
   <dimension ref="C3:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="40.77734375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="40.77734375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="C3" s="2" t="s">
+    <row r="3" spans="3:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="C3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C4" s="4" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D12" s="11"/>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D13" s="11"/>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D14" s="11"/>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C3:F3"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"NOK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1007,47 +1082,47 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="40.77734375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="40.77734375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="C3" s="2" t="s">
+    <row r="3" spans="3:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="C3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C4" s="4" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D12" s="11"/>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D13" s="11"/>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D14" s="11"/>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Popup update (Community creation and picture upload)
</commit_message>
<xml_diff>
--- a/SQL/PICTURA_SQLPlan.xlsx
+++ b/SQL/PICTURA_SQLPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephane\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HEIG-TIC\Git\BDR_Pictura\BDR_PICTURA\SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1202789B-FCF8-4E4F-86CA-9F00B92A0F5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AC8DCF-1E3F-4C5B-8AA5-243AE2E0E92C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SQLQueries" sheetId="1" r:id="rId1"/>
@@ -244,9 +244,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -273,6 +270,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -307,11 +307,11 @@
       <font>
         <b/>
         <i val="0"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF9F9F"/>
+          <bgColor rgb="FFB6DF89"/>
         </patternFill>
       </fill>
     </dxf>
@@ -319,11 +319,11 @@
       <font>
         <b/>
         <i val="0"/>
-        <color rgb="FF00B050"/>
+        <color rgb="FFFF0000"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFB6DF89"/>
+          <bgColor rgb="FFFF9F9F"/>
         </patternFill>
       </fill>
     </dxf>
@@ -635,48 +635,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="40.77734375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="40.77734375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="40.77734375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="40.77734375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="6" customWidth="1"/>
     <col min="6" max="6" width="10.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:6" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -684,13 +684,13 @@
       </c>
     </row>
     <row r="6" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -698,13 +698,13 @@
       </c>
     </row>
     <row r="7" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -712,13 +712,13 @@
       </c>
     </row>
     <row r="8" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -726,13 +726,13 @@
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -740,13 +740,13 @@
       </c>
     </row>
     <row r="10" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -754,13 +754,13 @@
       </c>
     </row>
     <row r="11" spans="3:6" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -768,13 +768,13 @@
       </c>
     </row>
     <row r="12" spans="3:6" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -782,13 +782,13 @@
       </c>
     </row>
     <row r="13" spans="3:6" ht="79.2" x14ac:dyDescent="0.3">
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -796,13 +796,13 @@
       </c>
     </row>
     <row r="14" spans="3:6" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -810,21 +810,21 @@
       </c>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -832,13 +832,13 @@
       </c>
     </row>
     <row r="17" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -846,13 +846,13 @@
       </c>
     </row>
     <row r="18" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -860,13 +860,13 @@
       </c>
     </row>
     <row r="19" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -874,13 +874,13 @@
       </c>
     </row>
     <row r="20" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F20" s="1" t="s">
@@ -888,13 +888,13 @@
       </c>
     </row>
     <row r="21" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -902,13 +902,13 @@
       </c>
     </row>
     <row r="22" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F22" s="1" t="s">
@@ -942,55 +942,55 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="40.77734375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="40.77734375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="40.77734375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="40.77734375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="6" customWidth="1"/>
     <col min="6" max="6" width="10.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:6" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D11" s="9"/>
+      <c r="D11" s="8"/>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D12" s="11"/>
+      <c r="D12" s="10"/>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D13" s="11"/>
+      <c r="D13" s="10"/>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D14" s="11"/>
+      <c r="D14" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C3:F3"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"NOK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1003,51 +1003,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF2D368-A179-4C7D-8F7E-AD97D2A718BC}">
   <dimension ref="C3:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="40.77734375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="40.77734375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="40.77734375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="40.77734375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="6" customWidth="1"/>
     <col min="6" max="6" width="10.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:6" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D11" s="9"/>
+      <c r="D11" s="8"/>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D12" s="11"/>
+      <c r="D12" s="10"/>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D13" s="11"/>
+      <c r="D13" s="10"/>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D14" s="11"/>
+      <c r="D14" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>